<commit_message>
Evaluations: #2, not sure what, but Excel file changed.
</commit_message>
<xml_diff>
--- a/eval/e2/texts.xlsx
+++ b/eval/e2/texts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="25080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Texts" sheetId="1" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>

</xml_diff>